<commit_message>
Ignore all xlsx files
</commit_message>
<xml_diff>
--- a/mttr_result.xlsx
+++ b/mttr_result.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>Issue Id</t>
   </si>
@@ -28,6 +28,414 @@
   </si>
   <si>
     <t>Time to Resolve In Seconds</t>
+  </si>
+  <si>
+    <t>155562014</t>
+  </si>
+  <si>
+    <t>resolved</t>
+  </si>
+  <si>
+    <t>Flasher</t>
+  </si>
+  <si>
+    <t>310.130000</t>
+  </si>
+  <si>
+    <t>151239531</t>
+  </si>
+  <si>
+    <t>1199289.562000</t>
+  </si>
+  <si>
+    <t>151228383</t>
+  </si>
+  <si>
+    <t>1201399.504000</t>
+  </si>
+  <si>
+    <t>152850359</t>
+  </si>
+  <si>
+    <t>Jesse Pinkman</t>
+  </si>
+  <si>
+    <t>61061.825000</t>
+  </si>
+  <si>
+    <t>152069770</t>
+  </si>
+  <si>
+    <t>256254.819000</t>
+  </si>
+  <si>
+    <t>151238703</t>
+  </si>
+  <si>
+    <t>509351.804000</t>
+  </si>
+  <si>
+    <t>151227403</t>
+  </si>
+  <si>
+    <t>511505.795000</t>
+  </si>
+  <si>
+    <t>169717015</t>
+  </si>
+  <si>
+    <t>Darth Vader</t>
+  </si>
+  <si>
+    <t>0.000000</t>
+  </si>
+  <si>
+    <t>170248393</t>
+  </si>
+  <si>
+    <t>104811.093000</t>
+  </si>
+  <si>
+    <t>164591448</t>
+  </si>
+  <si>
+    <t>169719925</t>
+  </si>
+  <si>
+    <t>62747.737000</t>
+  </si>
+  <si>
+    <t>169716789</t>
+  </si>
+  <si>
+    <t>63467.296000</t>
+  </si>
+  <si>
+    <t>169705049</t>
+  </si>
+  <si>
+    <t>66012.287000</t>
+  </si>
+  <si>
+    <t>164591458</t>
+  </si>
+  <si>
+    <t>1193684.219000</t>
+  </si>
+  <si>
+    <t>169702117</t>
+  </si>
+  <si>
+    <t>66691.264000</t>
+  </si>
+  <si>
+    <t>166092981</t>
+  </si>
+  <si>
+    <t>837003.249000</t>
+  </si>
+  <si>
+    <t>165066303</t>
+  </si>
+  <si>
+    <t>1099720.233000</t>
+  </si>
+  <si>
+    <t>162625833</t>
+  </si>
+  <si>
+    <t>162507821</t>
+  </si>
+  <si>
+    <t>34168.507000</t>
+  </si>
+  <si>
+    <t>157084177</t>
+  </si>
+  <si>
+    <t>157082777</t>
+  </si>
+  <si>
+    <t>157084423</t>
+  </si>
+  <si>
+    <t>145112.487000</t>
+  </si>
+  <si>
+    <t>157082602</t>
+  </si>
+  <si>
+    <t>145626.845000</t>
+  </si>
+  <si>
+    <t>151226916</t>
+  </si>
+  <si>
+    <t>3240213.388000</t>
+  </si>
+  <si>
+    <t>157574190</t>
+  </si>
+  <si>
+    <t>Yoda</t>
+  </si>
+  <si>
+    <t>488.081000</t>
+  </si>
+  <si>
+    <t>160844800</t>
+  </si>
+  <si>
+    <t>Arya</t>
+  </si>
+  <si>
+    <t>259.631000</t>
+  </si>
+  <si>
+    <t>160844619</t>
+  </si>
+  <si>
+    <t>295.618000</t>
+  </si>
+  <si>
+    <t>160412331</t>
+  </si>
+  <si>
+    <t>82632.604000</t>
+  </si>
+  <si>
+    <t>156436528</t>
+  </si>
+  <si>
+    <t>321981.234000</t>
+  </si>
+  <si>
+    <t>151240737</t>
+  </si>
+  <si>
+    <t>2687360.835000</t>
+  </si>
+  <si>
+    <t>151226076</t>
+  </si>
+  <si>
+    <t>2690233.791000</t>
+  </si>
+  <si>
+    <t>169615039</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>88379.044000</t>
+  </si>
+  <si>
+    <t>169614576</t>
+  </si>
+  <si>
+    <t>88449.038000</t>
+  </si>
+  <si>
+    <t>169606092</t>
+  </si>
+  <si>
+    <t>90093.031000</t>
+  </si>
+  <si>
+    <t>162599872</t>
+  </si>
+  <si>
+    <t>1544290.023000</t>
+  </si>
+  <si>
+    <t>162599057</t>
+  </si>
+  <si>
+    <t>1544529.014000</t>
+  </si>
+  <si>
+    <t>161067955</t>
+  </si>
+  <si>
+    <t>1917114.996000</t>
+  </si>
+  <si>
+    <t>161067568</t>
+  </si>
+  <si>
+    <t>1917180.980000</t>
+  </si>
+  <si>
+    <t>151238302</t>
+  </si>
+  <si>
+    <t>4773971.960000</t>
+  </si>
+  <si>
+    <t>151225222</t>
+  </si>
+  <si>
+    <t>4776496.947000</t>
+  </si>
+  <si>
+    <t>155295778</t>
+  </si>
+  <si>
+    <t>Brainiac</t>
+  </si>
+  <si>
+    <t>156680928</t>
+  </si>
+  <si>
+    <t>249616.670000</t>
+  </si>
+  <si>
+    <t>156502225</t>
+  </si>
+  <si>
+    <t>302184.090000</t>
+  </si>
+  <si>
+    <t>156412257</t>
+  </si>
+  <si>
+    <t>4187.692000</t>
+  </si>
+  <si>
+    <t>152945874</t>
+  </si>
+  <si>
+    <t>1019161.630000</t>
+  </si>
+  <si>
+    <t>153264405</t>
+  </si>
+  <si>
+    <t>950517.785000</t>
+  </si>
+  <si>
+    <t>153254996</t>
+  </si>
+  <si>
+    <t>952103.778000</t>
+  </si>
+  <si>
+    <t>153254864</t>
+  </si>
+  <si>
+    <t>952124.751000</t>
+  </si>
+  <si>
+    <t>153241223</t>
+  </si>
+  <si>
+    <t>954513.657000</t>
+  </si>
+  <si>
+    <t>153249007</t>
+  </si>
+  <si>
+    <t>953123.697000</t>
+  </si>
+  <si>
+    <t>153251199</t>
+  </si>
+  <si>
+    <t>952752.743000</t>
+  </si>
+  <si>
+    <t>153249313</t>
+  </si>
+  <si>
+    <t>953032.731000</t>
+  </si>
+  <si>
+    <t>153249286</t>
+  </si>
+  <si>
+    <t>953051.724000</t>
+  </si>
+  <si>
+    <t>153249132</t>
+  </si>
+  <si>
+    <t>953083.708000</t>
+  </si>
+  <si>
+    <t>153249060</t>
+  </si>
+  <si>
+    <t>953106.703000</t>
+  </si>
+  <si>
+    <t>153248900</t>
+  </si>
+  <si>
+    <t>953140.686000</t>
+  </si>
+  <si>
+    <t>153248444</t>
+  </si>
+  <si>
+    <t>953243.681000</t>
+  </si>
+  <si>
+    <t>153247875</t>
+  </si>
+  <si>
+    <t>953348.675000</t>
+  </si>
+  <si>
+    <t>153240855</t>
+  </si>
+  <si>
+    <t>954565.649000</t>
+  </si>
+  <si>
+    <t>153243820</t>
+  </si>
+  <si>
+    <t>954082.669000</t>
+  </si>
+  <si>
+    <t>153241893</t>
+  </si>
+  <si>
+    <t>954403.663000</t>
+  </si>
+  <si>
+    <t>153219462</t>
+  </si>
+  <si>
+    <t>958826.644000</t>
+  </si>
+  <si>
+    <t>153115277</t>
+  </si>
+  <si>
+    <t>979629.637000</t>
+  </si>
+  <si>
+    <t>151240203</t>
+  </si>
+  <si>
+    <t>1489641.621000</t>
+  </si>
+  <si>
+    <t>151225004</t>
+  </si>
+  <si>
+    <t>1492602.615000</t>
+  </si>
+  <si>
+    <t>156501291</t>
+  </si>
+  <si>
+    <t>Raiden</t>
+  </si>
+  <si>
+    <t>302507.986000</t>
   </si>
 </sst>
 </file>
@@ -397,7 +805,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -425,6 +833,930 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>